<commit_message>
added new testcase 'TC_ProjectDropdownTopics'
</commit_message>
<xml_diff>
--- a/src/test/java/com/DemoGuru/testData/DDTdata.xlsx
+++ b/src/test/java/com/DemoGuru/testData/DDTdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23895" windowHeight="9990"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="23895" windowHeight="9990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ProjectDDs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -382,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -449,35 +449,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>12632</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new testcase InsuranceRegisterTest and minor enhancements
</commit_message>
<xml_diff>
--- a/src/test/java/com/DemoGuru/testData/DDTdata.xlsx
+++ b/src/test/java/com/DemoGuru/testData/DDTdata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23895" windowHeight="9990" activeTab="1"/>
+    <workbookView activeTab="3" windowHeight="9990" windowWidth="23895" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="ProjectDDs" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="ProjectDDs" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Emails" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -40,12 +41,22 @@
   </si>
   <si>
     <t>hYjemEt</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>word 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">word 2 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -80,18 +91,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -100,10 +111,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -259,7 +270,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -268,13 +279,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -284,7 +295,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -293,7 +304,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -302,7 +313,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -312,12 +323,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -348,7 +359,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -367,7 +378,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -380,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
@@ -388,7 +399,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -440,27 +451,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1"/>
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1"/>
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2">
@@ -468,18 +483,84 @@
       <c r="B3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E5:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>